<commit_message>
Popravljen OdabirRestorana pdf, detaljnije urađen glavni uml
</commit_message>
<xml_diff>
--- a/UseCaseIScenarij/OdabirRestorana.xlsx
+++ b/UseCaseIScenarij/OdabirRestorana.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
   <si>
     <t>Naziv</t>
   </si>
@@ -109,9 +109,6 @@
   </si>
   <si>
     <t>2. Prikaz forme pretrage restorana</t>
-  </si>
-  <si>
-    <t>Izbor (eng. Confirmation), odnosno odustajanje od potrage, željenog restorana od više ponuđenih, te dobijanje uputa za izabrani restoran.</t>
   </si>
   <si>
     <t>Imati instaliranu aplikaciju i kliknuti opciju za pretragu restorana.</t>
@@ -626,8 +623,8 @@
   </sheetPr>
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -663,12 +660,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -676,7 +673,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -684,7 +681,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -808,7 +805,7 @@
     </row>
     <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>

</xml_diff>

<commit_message>
Update OdabirRestorana i Vicinor uml
</commit_message>
<xml_diff>
--- a/UseCaseIScenarij/OdabirRestorana.xlsx
+++ b/UseCaseIScenarij/OdabirRestorana.xlsx
@@ -96,9 +96,6 @@
     <t>Odabir restorana (vicinor app)</t>
   </si>
   <si>
-    <t>3. Prikaz liste svih ponuđenih restorana na osnovu ispunjenih podataka</t>
-  </si>
-  <si>
     <t>6. Korištenje GPS za direkcije</t>
   </si>
   <si>
@@ -118,6 +115,9 @@
   </si>
   <si>
     <t>Alternativni tok, ako korisnik ne odabere restoran:</t>
+  </si>
+  <si>
+    <t>3. Prikaz liste svih ponuđenih restorana na osnovu ispunjenih podataka, pri čemu ukoliko je dati restoran među omiljenim drugačije je naznačen u odnosu na ostale</t>
   </si>
 </sst>
 </file>
@@ -624,7 +624,7 @@
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -673,7 +673,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -681,7 +681,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -758,10 +758,10 @@
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
     </row>
-    <row r="24" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="5"/>
       <c r="C24" s="5" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="D24" s="5"/>
     </row>
@@ -783,13 +783,13 @@
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="5"/>
       <c r="C28" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D28" s="5"/>
     </row>
@@ -805,7 +805,7 @@
     </row>
     <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -824,7 +824,7 @@
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
@@ -832,7 +832,7 @@
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" s="5"/>
       <c r="C34" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D34" s="5"/>
     </row>

</xml_diff>